<commit_message>
Phase 1 now emits an equipment list. This is helpful for mocking Phase2 data. Work adding modem to the Outstation template.
</commit_message>
<xml_diff>
--- a/OutstationPatcher/excel-sample/OS_Worklist_Sample.xlsx
+++ b/OutstationPatcher/excel-sample/OS_Worklist_Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-patch\OutstationPatcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406451BC-5AAB-434C-82BB-9A41793AEA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C7F585-852D-4FC6-934B-2B4F23A62508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{65655A23-1E29-4E70-A082-B5F633D8CB57}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
   <si>
     <t>AI2 Equipment PLI Code</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>S4 System Code</t>
+  </si>
+  <si>
+    <t>Modem Name</t>
+  </si>
+  <si>
+    <t>Modem</t>
   </si>
 </sst>
 </file>
@@ -725,12 +731,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83161465-1FCA-41A2-BCF2-D6E72ABABA7E}">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,16 +756,17 @@
     <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.5703125" customWidth="1"/>
-    <col min="21" max="21" width="25.140625" customWidth="1"/>
-    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.5703125" customWidth="1"/>
-    <col min="24" max="24" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="52" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5703125" customWidth="1"/>
+    <col min="20" max="20" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" customWidth="1"/>
+    <col min="25" max="25" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -815,28 +822,31 @@
         <v>19</v>
       </c>
       <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -892,28 +902,31 @@
         <v>91</v>
       </c>
       <c r="S2" t="s">
+        <v>110</v>
+      </c>
+      <c r="T2" t="s">
         <v>89</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>88</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>106</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <v>43836</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>15</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -951,25 +964,28 @@
         <v>91</v>
       </c>
       <c r="S3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T3" t="s">
         <v>89</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>88</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>106</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1">
         <v>43668</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1025,25 +1041,28 @@
         <v>91</v>
       </c>
       <c r="S4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T4" t="s">
         <v>89</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>88</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>106</v>
       </c>
-      <c r="W4" s="1">
+      <c r="X4" s="1">
         <v>43683</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1099,26 +1118,29 @@
         <v>91</v>
       </c>
       <c r="S5" t="s">
+        <v>110</v>
+      </c>
+      <c r="T5" t="s">
         <v>86</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>87</v>
       </c>
-      <c r="U5" s="3"/>
-      <c r="V5" t="s">
+      <c r="V5" s="3"/>
+      <c r="W5" t="s">
         <v>106</v>
       </c>
-      <c r="W5" s="1">
+      <c r="X5" s="1">
         <v>43684</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>15</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1156,25 +1178,28 @@
         <v>91</v>
       </c>
       <c r="S6" t="s">
+        <v>110</v>
+      </c>
+      <c r="T6" t="s">
         <v>89</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>88</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="V6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>106</v>
       </c>
-      <c r="W6" s="1">
+      <c r="X6" s="1">
         <v>43684</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1230,25 +1255,28 @@
         <v>91</v>
       </c>
       <c r="S7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T7" t="s">
         <v>89</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>88</v>
       </c>
-      <c r="U7" s="3" t="s">
+      <c r="V7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>106</v>
       </c>
-      <c r="W7" s="1">
+      <c r="X7" s="1">
         <v>43710</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1304,28 +1332,31 @@
         <v>91</v>
       </c>
       <c r="S8" t="s">
+        <v>110</v>
+      </c>
+      <c r="T8" t="s">
         <v>89</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>88</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="V8" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>106</v>
       </c>
-      <c r="W8" s="1">
+      <c r="X8" s="1">
         <v>43711</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>15</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1363,25 +1394,28 @@
         <v>91</v>
       </c>
       <c r="S9" t="s">
+        <v>110</v>
+      </c>
+      <c r="T9" t="s">
         <v>89</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>88</v>
       </c>
-      <c r="U9" s="3" t="s">
+      <c r="V9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>106</v>
       </c>
-      <c r="W9" s="1">
+      <c r="X9" s="1">
         <v>43712</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1437,28 +1471,31 @@
         <v>91</v>
       </c>
       <c r="S10" t="s">
+        <v>110</v>
+      </c>
+      <c r="T10" t="s">
         <v>89</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>88</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="V10" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>106</v>
       </c>
-      <c r="W10" s="1">
+      <c r="X10" s="1">
         <v>43717</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>15</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1514,24 +1551,27 @@
         <v>91</v>
       </c>
       <c r="S11" t="s">
+        <v>110</v>
+      </c>
+      <c r="T11" t="s">
         <v>86</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>87</v>
       </c>
-      <c r="U11" s="3" t="s">
+      <c r="V11" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>106</v>
       </c>
-      <c r="W11" s="1">
+      <c r="X11" s="1">
         <v>43717</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>15</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Work on memo lines. Should now be visible to the Outstation Patcher.
</commit_message>
<xml_diff>
--- a/OutstationPatcher/excel-sample/OS_Worklist_Sample.xlsx
+++ b/OutstationPatcher/excel-sample/OS_Worklist_Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-patch\OutstationPatcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C7F585-852D-4FC6-934B-2B4F23A62508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF41AC56-65F2-495F-BE84-00D2BE07485A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{65655A23-1E29-4E70-A082-B5F633D8CB57}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="114">
   <si>
     <t>AI2 Equipment PLI Code</t>
   </si>
@@ -69,9 +69,6 @@
     <t>MMIM</t>
   </si>
   <si>
-    <t>Oustation Serial Number</t>
-  </si>
-  <si>
     <t>AI2 NET Sainum</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Adding below system so don't need AI2 CAA Sainum etc.</t>
   </si>
   <si>
-    <t>Oustation Specific Model</t>
-  </si>
-  <si>
     <t>Outstation Install Date</t>
   </si>
   <si>
@@ -364,6 +358,21 @@
   </si>
   <si>
     <t>Modem</t>
+  </si>
+  <si>
+    <t>Modem Memo Line</t>
+  </si>
+  <si>
+    <t>Installed Summer 2019</t>
+  </si>
+  <si>
+    <t>Outstation Memo Line</t>
+  </si>
+  <si>
+    <t>Outstation Specific Model</t>
+  </si>
+  <si>
+    <t>Outstation Serial Number</t>
   </si>
 </sst>
 </file>
@@ -731,12 +740,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83161465-1FCA-41A2-BCF2-D6E72ABABA7E}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,17 +765,18 @@
     <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.5703125" customWidth="1"/>
-    <col min="20" max="20" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.5703125" customWidth="1"/>
-    <col min="22" max="22" width="25.140625" customWidth="1"/>
-    <col min="23" max="23" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.5703125" customWidth="1"/>
-    <col min="25" max="25" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="52" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="23.5703125" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.5703125" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" customWidth="1"/>
+    <col min="24" max="24" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" customWidth="1"/>
+    <col min="26" max="26" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.85546875" customWidth="1"/>
+    <col min="28" max="28" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -777,16 +787,16 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -795,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
@@ -804,10 +814,10 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O1" t="s">
         <v>8</v>
@@ -816,69 +826,75 @@
         <v>9</v>
       </c>
       <c r="Q1" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="R1" t="s">
+        <v>112</v>
+      </c>
+      <c r="S1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" t="s">
+        <v>107</v>
+      </c>
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" t="s">
         <v>109</v>
       </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L2" t="s">
         <v>10</v>
@@ -890,57 +906,63 @@
         <v>7.5</v>
       </c>
       <c r="O2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P2" t="s">
         <v>11</v>
       </c>
       <c r="Q2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S2" t="s">
         <v>110</v>
       </c>
       <c r="T2" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="U2" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" t="s">
+        <v>86</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="W2" t="s">
-        <v>106</v>
-      </c>
-      <c r="X2" s="1">
+      <c r="X2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y2" s="1">
         <v>43836</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>15</v>
       </c>
-      <c r="Z2" t="s">
-        <v>18</v>
+      <c r="AA2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
         <v>10</v>
@@ -952,72 +974,78 @@
         <v>7.5</v>
       </c>
       <c r="O3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P3" t="s">
         <v>11</v>
       </c>
       <c r="Q3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S3" t="s">
         <v>110</v>
       </c>
       <c r="T3" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="U3" t="s">
-        <v>88</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="W3" t="s">
-        <v>106</v>
-      </c>
-      <c r="X3" s="1">
+        <v>87</v>
+      </c>
+      <c r="V3" t="s">
+        <v>86</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y3" s="1">
         <v>43668</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>15</v>
       </c>
+      <c r="AA3" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>54</v>
       </c>
-      <c r="F4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" t="s">
-        <v>56</v>
-      </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L4" t="s">
         <v>10</v>
@@ -1029,72 +1057,78 @@
         <v>7.5</v>
       </c>
       <c r="O4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P4" t="s">
         <v>11</v>
       </c>
       <c r="Q4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="R4" t="s">
+        <v>89</v>
+      </c>
+      <c r="S4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T4" t="s">
+        <v>108</v>
+      </c>
+      <c r="U4" t="s">
+        <v>87</v>
+      </c>
+      <c r="V4" t="s">
+        <v>86</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="S4" t="s">
-        <v>110</v>
-      </c>
-      <c r="T4" t="s">
-        <v>89</v>
-      </c>
-      <c r="U4" t="s">
-        <v>88</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="W4" t="s">
-        <v>106</v>
-      </c>
-      <c r="X4" s="1">
+      <c r="X4" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y4" s="1">
         <v>43683</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>15</v>
       </c>
+      <c r="AA4" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
       <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>58</v>
       </c>
-      <c r="F5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" t="s">
-        <v>60</v>
-      </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L5" t="s">
         <v>10</v>
@@ -1106,55 +1140,61 @@
         <v>7.5</v>
       </c>
       <c r="O5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P5" t="s">
         <v>11</v>
       </c>
       <c r="Q5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S5" t="s">
         <v>110</v>
       </c>
       <c r="T5" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="U5" t="s">
-        <v>87</v>
-      </c>
-      <c r="V5" s="3"/>
-      <c r="W5" t="s">
-        <v>106</v>
-      </c>
-      <c r="X5" s="1">
+        <v>84</v>
+      </c>
+      <c r="V5" t="s">
+        <v>85</v>
+      </c>
+      <c r="W5" s="3"/>
+      <c r="X5" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y5" s="1">
         <v>43684</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>15</v>
       </c>
-      <c r="Z5" t="s">
-        <v>17</v>
+      <c r="AA5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L6" t="s">
         <v>10</v>
@@ -1166,72 +1206,78 @@
         <v>7.5</v>
       </c>
       <c r="O6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P6" t="s">
         <v>11</v>
       </c>
       <c r="Q6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="R6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S6" t="s">
         <v>110</v>
       </c>
       <c r="T6" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="U6" t="s">
-        <v>88</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="W6" t="s">
-        <v>106</v>
-      </c>
-      <c r="X6" s="1">
+        <v>87</v>
+      </c>
+      <c r="V6" t="s">
+        <v>86</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="X6" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y6" s="1">
         <v>43684</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>15</v>
       </c>
+      <c r="AA6" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
       <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
         <v>61</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>62</v>
       </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
-      </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" t="s">
         <v>100</v>
       </c>
-      <c r="J7" t="s">
-        <v>102</v>
-      </c>
       <c r="K7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L7" t="s">
         <v>10</v>
@@ -1243,72 +1289,78 @@
         <v>7.5</v>
       </c>
       <c r="O7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P7" t="s">
         <v>11</v>
       </c>
       <c r="Q7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="R7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S7" t="s">
         <v>110</v>
       </c>
       <c r="T7" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="U7" t="s">
-        <v>88</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="W7" t="s">
-        <v>106</v>
-      </c>
-      <c r="X7" s="1">
+        <v>87</v>
+      </c>
+      <c r="V7" t="s">
+        <v>86</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="X7" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y7" s="1">
         <v>43710</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>15</v>
       </c>
+      <c r="AA7" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L8" t="s">
         <v>10</v>
@@ -1320,57 +1372,63 @@
         <v>7.5</v>
       </c>
       <c r="O8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P8" t="s">
         <v>11</v>
       </c>
       <c r="Q8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S8" t="s">
         <v>110</v>
       </c>
       <c r="T8" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="U8" t="s">
-        <v>88</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="W8" t="s">
-        <v>106</v>
-      </c>
-      <c r="X8" s="1">
+        <v>87</v>
+      </c>
+      <c r="V8" t="s">
+        <v>86</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="X8" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y8" s="1">
         <v>43711</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>15</v>
       </c>
-      <c r="Z8" t="s">
-        <v>17</v>
+      <c r="AA8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L9" t="s">
         <v>10</v>
@@ -1382,72 +1440,78 @@
         <v>7.5</v>
       </c>
       <c r="O9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P9" t="s">
         <v>11</v>
       </c>
       <c r="Q9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S9" t="s">
         <v>110</v>
       </c>
       <c r="T9" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="U9" t="s">
-        <v>88</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="W9" t="s">
-        <v>106</v>
-      </c>
-      <c r="X9" s="1">
+        <v>87</v>
+      </c>
+      <c r="V9" t="s">
+        <v>86</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="X9" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y9" s="1">
         <v>43712</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>15</v>
       </c>
+      <c r="AA9" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
         <v>67</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>69</v>
       </c>
-      <c r="F10" t="s">
-        <v>71</v>
-      </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L10" t="s">
         <v>10</v>
@@ -1459,75 +1523,81 @@
         <v>7.5</v>
       </c>
       <c r="O10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P10" t="s">
         <v>11</v>
       </c>
       <c r="Q10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="R10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S10" t="s">
         <v>110</v>
       </c>
       <c r="T10" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="U10" t="s">
-        <v>88</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="W10" t="s">
-        <v>106</v>
-      </c>
-      <c r="X10" s="1">
+        <v>87</v>
+      </c>
+      <c r="V10" t="s">
+        <v>86</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="X10" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y10" s="1">
         <v>43717</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>15</v>
       </c>
-      <c r="Z10" t="s">
-        <v>17</v>
+      <c r="AA10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
       <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
         <v>68</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>70</v>
       </c>
-      <c r="F11" t="s">
-        <v>72</v>
-      </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L11" t="s">
         <v>10</v>
@@ -1539,40 +1609,46 @@
         <v>7.5</v>
       </c>
       <c r="O11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P11" t="s">
         <v>11</v>
       </c>
       <c r="Q11" t="s">
+        <v>83</v>
+      </c>
+      <c r="R11" t="s">
+        <v>89</v>
+      </c>
+      <c r="S11" t="s">
+        <v>110</v>
+      </c>
+      <c r="T11" t="s">
+        <v>108</v>
+      </c>
+      <c r="U11" t="s">
+        <v>84</v>
+      </c>
+      <c r="V11" t="s">
         <v>85</v>
       </c>
-      <c r="R11" t="s">
-        <v>91</v>
-      </c>
-      <c r="S11" t="s">
-        <v>110</v>
-      </c>
-      <c r="T11" t="s">
-        <v>86</v>
-      </c>
-      <c r="U11" t="s">
-        <v>87</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W11" t="s">
-        <v>106</v>
-      </c>
-      <c r="X11" s="1">
+      <c r="W11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="X11" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y11" s="1">
         <v>43717</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>15</v>
       </c>
-      <c r="Z11" t="s">
-        <v>17</v>
+      <c r="AA11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes to get Oustation Patcher working again.
</commit_message>
<xml_diff>
--- a/OutstationPatcher/excel-sample/OS_Worklist_Sample.xlsx
+++ b/OutstationPatcher/excel-sample/OS_Worklist_Sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-patch\OutstationPatcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF41AC56-65F2-495F-BE84-00D2BE07485A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2FBC40-69B4-4DFB-BD83-C1CEFBF7A494}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{65655A23-1E29-4E70-A082-B5F633D8CB57}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="112">
   <si>
     <t>AI2 Equipment PLI Code</t>
   </si>
@@ -97,12 +97,6 @@
   </si>
   <si>
     <t>Modem Install Date</t>
-  </si>
-  <si>
-    <t>Modem Asset Life (Years)</t>
-  </si>
-  <si>
-    <t>Outstation Asset Life (Years)</t>
   </si>
   <si>
     <t>SAI00228537</t>
@@ -420,10 +414,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -740,12 +733,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83161465-1FCA-41A2-BCF2-D6E72ABABA7E}">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,23 +753,21 @@
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.140625" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="23.5703125" customWidth="1"/>
-    <col min="21" max="21" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.5703125" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" customWidth="1"/>
-    <col min="24" max="24" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" customWidth="1"/>
-    <col min="26" max="26" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.85546875" customWidth="1"/>
-    <col min="28" max="28" width="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="23.5703125" customWidth="1"/>
+    <col min="20" max="20" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" customWidth="1"/>
+    <col min="25" max="25" width="23.85546875" customWidth="1"/>
+    <col min="26" max="26" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
@@ -817,84 +808,78 @@
         <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P1" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="Q1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="S1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
         <v>107</v>
       </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>46</v>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L2" t="s">
         <v>10</v>
@@ -902,67 +887,61 @@
       <c r="M2" s="1">
         <v>43836</v>
       </c>
-      <c r="N2" s="2">
-        <v>7.5</v>
+      <c r="N2" t="s">
+        <v>71</v>
       </c>
       <c r="O2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P2" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="Q2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="R2" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="S2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T2" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="U2" t="s">
-        <v>87</v>
-      </c>
-      <c r="V2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="X2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y2" s="1">
+      <c r="W2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X2" s="1">
         <v>43836</v>
       </c>
-      <c r="Z2">
-        <v>15</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="Y2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L3" t="s">
         <v>10</v>
@@ -970,82 +949,76 @@
       <c r="M3" s="1">
         <v>43668</v>
       </c>
-      <c r="N3">
-        <v>7.5</v>
+      <c r="N3" t="s">
+        <v>71</v>
       </c>
       <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
         <v>73</v>
       </c>
-      <c r="P3" t="s">
-        <v>11</v>
-      </c>
       <c r="Q3" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="R3" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="S3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T3" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="U3" t="s">
-        <v>87</v>
-      </c>
-      <c r="V3" t="s">
-        <v>86</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="X3" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y3" s="1">
+        <v>84</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="W3" t="s">
+        <v>102</v>
+      </c>
+      <c r="X3" s="1">
         <v>43668</v>
       </c>
-      <c r="Z3">
-        <v>15</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>110</v>
+      <c r="Y3" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>52</v>
       </c>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
-      </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L4" t="s">
         <v>10</v>
@@ -1053,82 +1026,76 @@
       <c r="M4" s="1">
         <v>43683</v>
       </c>
-      <c r="N4">
-        <v>7.5</v>
+      <c r="N4" t="s">
+        <v>71</v>
       </c>
       <c r="O4" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P4" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="Q4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="R4" t="s">
+        <v>108</v>
+      </c>
+      <c r="S4" t="s">
+        <v>106</v>
+      </c>
+      <c r="T4" t="s">
+        <v>85</v>
+      </c>
+      <c r="U4" t="s">
+        <v>84</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S4" t="s">
-        <v>110</v>
-      </c>
-      <c r="T4" t="s">
-        <v>108</v>
-      </c>
-      <c r="U4" t="s">
-        <v>87</v>
-      </c>
-      <c r="V4" t="s">
-        <v>86</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="X4" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y4" s="1">
+      <c r="W4" t="s">
+        <v>102</v>
+      </c>
+      <c r="X4" s="1">
         <v>43683</v>
       </c>
-      <c r="Z4">
-        <v>15</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>110</v>
+      <c r="Y4" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
       <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>56</v>
       </c>
-      <c r="F5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" t="s">
-        <v>58</v>
-      </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L5" t="s">
         <v>10</v>
@@ -1136,65 +1103,59 @@
       <c r="M5" s="1">
         <v>43684</v>
       </c>
-      <c r="N5">
-        <v>7.5</v>
+      <c r="N5" t="s">
+        <v>71</v>
       </c>
       <c r="O5" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P5" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="Q5" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="R5" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="S5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T5" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="U5" t="s">
-        <v>84</v>
-      </c>
-      <c r="V5" t="s">
-        <v>85</v>
-      </c>
-      <c r="W5" s="3"/>
-      <c r="X5" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y5" s="1">
+        <v>83</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" t="s">
+        <v>102</v>
+      </c>
+      <c r="X5" s="1">
         <v>43684</v>
       </c>
-      <c r="Z5">
-        <v>15</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB5" t="s">
+      <c r="Y5" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L6" t="s">
         <v>10</v>
@@ -1202,82 +1163,76 @@
       <c r="M6" s="1">
         <v>43684</v>
       </c>
-      <c r="N6">
-        <v>7.5</v>
+      <c r="N6" t="s">
+        <v>71</v>
       </c>
       <c r="O6" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P6" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="Q6" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="R6" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="S6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T6" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="U6" t="s">
-        <v>87</v>
-      </c>
-      <c r="V6" t="s">
-        <v>86</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="X6" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y6" s="1">
+        <v>84</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="W6" t="s">
+        <v>102</v>
+      </c>
+      <c r="X6" s="1">
         <v>43684</v>
       </c>
-      <c r="Z6">
-        <v>15</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>110</v>
+      <c r="Y6" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
       <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
         <v>59</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="F7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" t="s">
-        <v>62</v>
-      </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" t="s">
         <v>98</v>
       </c>
-      <c r="J7" t="s">
-        <v>100</v>
-      </c>
       <c r="K7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L7" t="s">
         <v>10</v>
@@ -1285,82 +1240,76 @@
       <c r="M7" s="1">
         <v>43710</v>
       </c>
-      <c r="N7">
-        <v>7.5</v>
+      <c r="N7" t="s">
+        <v>71</v>
       </c>
       <c r="O7" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P7" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="Q7" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="R7" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="S7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T7" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="U7" t="s">
-        <v>87</v>
-      </c>
-      <c r="V7" t="s">
-        <v>86</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="X7" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y7" s="1">
+        <v>84</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="W7" t="s">
+        <v>102</v>
+      </c>
+      <c r="X7" s="1">
         <v>43710</v>
       </c>
-      <c r="Z7">
-        <v>15</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>110</v>
+      <c r="Y7" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L8" t="s">
         <v>10</v>
@@ -1368,67 +1317,61 @@
       <c r="M8" s="1">
         <v>43711</v>
       </c>
-      <c r="N8">
-        <v>7.5</v>
+      <c r="N8" t="s">
+        <v>71</v>
       </c>
       <c r="O8" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P8" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="Q8" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="R8" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="S8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T8" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="U8" t="s">
-        <v>87</v>
-      </c>
-      <c r="V8" t="s">
-        <v>86</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="X8" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y8" s="1">
+        <v>84</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="W8" t="s">
+        <v>102</v>
+      </c>
+      <c r="X8" s="1">
         <v>43711</v>
       </c>
-      <c r="Z8">
-        <v>15</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB8" t="s">
+      <c r="Y8" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L9" t="s">
         <v>10</v>
@@ -1436,82 +1379,76 @@
       <c r="M9" s="1">
         <v>43712</v>
       </c>
-      <c r="N9">
-        <v>7.5</v>
+      <c r="N9" t="s">
+        <v>71</v>
       </c>
       <c r="O9" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P9" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="Q9" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="R9" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="S9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T9" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="U9" t="s">
-        <v>87</v>
-      </c>
-      <c r="V9" t="s">
-        <v>86</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="X9" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y9" s="1">
+        <v>84</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="W9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X9" s="1">
         <v>43712</v>
       </c>
-      <c r="Z9">
-        <v>15</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>110</v>
+      <c r="Y9" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
         <v>65</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>67</v>
       </c>
-      <c r="F10" t="s">
-        <v>69</v>
-      </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L10" t="s">
         <v>10</v>
@@ -1519,85 +1456,79 @@
       <c r="M10" s="1">
         <v>43717</v>
       </c>
-      <c r="N10">
-        <v>7.5</v>
+      <c r="N10" t="s">
+        <v>71</v>
       </c>
       <c r="O10" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P10" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="Q10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="R10" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="S10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T10" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="U10" t="s">
-        <v>87</v>
-      </c>
-      <c r="V10" t="s">
-        <v>86</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="X10" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y10" s="1">
+        <v>84</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="W10" t="s">
+        <v>102</v>
+      </c>
+      <c r="X10" s="1">
         <v>43717</v>
       </c>
-      <c r="Z10">
-        <v>15</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB10" t="s">
+      <c r="Y10" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
       <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
         <v>66</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>68</v>
       </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L11" t="s">
         <v>10</v>
@@ -1605,49 +1536,43 @@
       <c r="M11" s="1">
         <v>43717</v>
       </c>
-      <c r="N11">
-        <v>7.5</v>
+      <c r="N11" t="s">
+        <v>71</v>
       </c>
       <c r="O11" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="P11" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="Q11" t="s">
+        <v>87</v>
+      </c>
+      <c r="R11" t="s">
+        <v>108</v>
+      </c>
+      <c r="S11" t="s">
+        <v>106</v>
+      </c>
+      <c r="T11" t="s">
+        <v>82</v>
+      </c>
+      <c r="U11" t="s">
         <v>83</v>
       </c>
-      <c r="R11" t="s">
-        <v>89</v>
-      </c>
-      <c r="S11" t="s">
-        <v>110</v>
-      </c>
-      <c r="T11" t="s">
-        <v>108</v>
-      </c>
-      <c r="U11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V11" t="s">
-        <v>85</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="X11" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y11" s="1">
+      <c r="V11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W11" t="s">
+        <v>102</v>
+      </c>
+      <c r="X11" s="1">
         <v>43717</v>
       </c>
-      <c r="Z11">
-        <v>15</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB11" t="s">
+      <c r="Y11" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z11" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>